<commit_message>
feat: improve audio and background generators; enhance character command formatting; update text generator printer handling; update Excel files on Naninovel verision
</commit_message>
<xml_diff>
--- a/param_config/param_data_naninovel.xlsx
+++ b/param_config/param_data_naninovel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\视觉小说项目\【表格演出工具】重制版\param_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\视觉小说项目\【表格演出工具】git仓库\param_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFC204F-4327-4A15-B704-22D685A80843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A4512-1278-4E08-A17B-7EFE90C261AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="8" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
   <si>
     <t>ExcelParam</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -286,26 +286,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>@despawn Blur</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>取消模糊</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>@spawn ShakeCamera params:,3,,,0.8,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大震动</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>@spawn ShakeCamera params:,2,,,0.4,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>小震动</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -379,6 +367,34 @@
   </si>
   <si>
     <t>the_printer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姿势变换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the_pose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>色调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the_tint_color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@spawn ShakeCamera params:,2,,,0.3,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@spawn ShakeCamera params:,3,,,0.6,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@blur power:0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1093,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1115,25 +1131,33 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1146,7 +1170,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE18EF0-AEBE-4348-BCBF-A1A94009AC4C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -1168,18 +1192,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1287,10 +1319,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1463,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF8993-2144-488C-A876-54C4032DB63D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1483,10 +1515,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,18 +1531,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1598,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A521C93D-9983-4554-8EB8-0FE7DA0F0FDA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1618,26 +1650,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1671,18 +1703,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1716,34 +1748,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: integrate ExcelFileManager and DataFrameProcessor for improved Excel handling and data processing feat&fix: improve Excel params and fix generate logic in Naninovel
</commit_message>
<xml_diff>
--- a/param_config/param_data_naninovel.xlsx
+++ b/param_config/param_data_naninovel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\视觉小说项目\【表格演出工具】git仓库\param_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\视觉小说项目\【表格演出工具】dev\param_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A4512-1278-4E08-A17B-7EFE90C261AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A77C839-8678-46CA-9BAB-983CD2A7D98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Background" sheetId="6" r:id="rId7"/>
     <sheet name="Event" sheetId="7" r:id="rId8"/>
     <sheet name="Id" sheetId="1" r:id="rId9"/>
-    <sheet name="Speaker" sheetId="5" r:id="rId10"/>
+    <sheet name="Name" sheetId="5" r:id="rId10"/>
     <sheet name="Character" sheetId="11" r:id="rId11"/>
     <sheet name="Varient" sheetId="16" r:id="rId12"/>
     <sheet name="Pose" sheetId="2" r:id="rId13"/>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5E86-0F35-431D-B760-B491C7011A1E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1630,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A521C93D-9983-4554-8EB8-0FE7DA0F0FDA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>